<commit_message>
Re-saved Images - realized I was overwriting...
</commit_message>
<xml_diff>
--- a/PredictionData/accuracy.xlsx
+++ b/PredictionData/accuracy.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/annmcnamara/Project_3/PredictionData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A42E6CF1-96EB-0347-9F5D-52AC8D58AAD2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56A56005-A86D-354A-8EB7-3C71CA54720C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5920" yWindow="3860" windowWidth="23240" windowHeight="11440" xr2:uid="{C081B34F-8AB1-DD45-ABE6-DBA21B89C5F3}"/>
+    <workbookView xWindow="5920" yWindow="3540" windowWidth="23240" windowHeight="11440" xr2:uid="{C081B34F-8AB1-DD45-ABE6-DBA21B89C5F3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -70,7 +70,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -83,6 +83,11 @@
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Arial Bold"/>
     </font>
   </fonts>
   <fills count="3">
@@ -135,11 +140,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -457,17 +462,17 @@
   <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="39.33203125" customWidth="1"/>
-    <col min="2" max="2" width="27.33203125" customWidth="1"/>
-    <col min="3" max="3" width="25.33203125" customWidth="1"/>
+    <col min="2" max="2" width="28.5" customWidth="1"/>
+    <col min="3" max="3" width="28.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="48" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" ht="48" customHeight="1">
       <c r="A1" s="4" t="s">
         <v>9</v>
       </c>
@@ -481,19 +486,19 @@
       <c r="E1" s="3"/>
       <c r="F1" s="3"/>
     </row>
-    <row r="2" spans="1:6" ht="20" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" ht="20">
       <c r="A2" s="5" t="s">
         <v>6</v>
       </c>
       <c r="B2" s="6">
-        <v>0.96998664280961799</v>
+        <v>0.94168022772396498</v>
       </c>
       <c r="C2" s="6">
-        <v>0.85854051552522204</v>
+        <v>0.85767991774849295</v>
       </c>
       <c r="D2" s="1"/>
     </row>
-    <row r="3" spans="1:6" ht="20" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" ht="20">
       <c r="A3" s="5" t="s">
         <v>7</v>
       </c>
@@ -501,11 +506,11 @@
         <v>0.99113993917319398</v>
       </c>
       <c r="C3" s="6">
-        <v>0.99113993917319398</v>
+        <v>0.97443231131058194</v>
       </c>
       <c r="D3" s="1"/>
     </row>
-    <row r="4" spans="1:6" ht="20" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" ht="20">
       <c r="A4" s="5" t="s">
         <v>1</v>
       </c>
@@ -517,19 +522,19 @@
       </c>
       <c r="D4" s="1"/>
     </row>
-    <row r="5" spans="1:6" ht="20" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" ht="20">
       <c r="A5" s="5" t="s">
         <v>4</v>
       </c>
       <c r="B5" s="6">
-        <v>0.95191111580108401</v>
+        <v>0.95064518344011095</v>
       </c>
       <c r="C5" s="6">
         <v>0.99122232790950504</v>
       </c>
       <c r="D5" s="1"/>
     </row>
-    <row r="6" spans="1:6" ht="20" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" ht="20">
       <c r="A6" s="5" t="s">
         <v>3</v>
       </c>
@@ -541,31 +546,31 @@
       </c>
       <c r="D6" s="1"/>
     </row>
-    <row r="7" spans="1:6" ht="20" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" ht="20">
       <c r="A7" s="5" t="s">
         <v>8</v>
       </c>
       <c r="B7" s="6">
-        <v>0.82432966048949796</v>
+        <v>0.915665050232775</v>
       </c>
       <c r="C7" s="6">
-        <v>0.96428647618958996</v>
+        <v>0.96511703800835902</v>
       </c>
       <c r="D7" s="1"/>
     </row>
-    <row r="8" spans="1:6" ht="20" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" ht="20">
       <c r="A8" s="5" t="s">
         <v>0</v>
       </c>
       <c r="B8" s="6">
-        <v>0.96751263714015201</v>
+        <v>0.88348743566452104</v>
       </c>
       <c r="C8" s="6">
         <v>0.97603605814002703</v>
       </c>
       <c r="D8" s="1"/>
     </row>
-    <row r="9" spans="1:6" ht="20" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" ht="20">
       <c r="A9" s="5" t="s">
         <v>2</v>
       </c>
@@ -577,19 +582,19 @@
       </c>
       <c r="D9" s="1"/>
     </row>
-    <row r="10" spans="1:6" ht="20" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" ht="20">
       <c r="A10" s="5" t="s">
         <v>5</v>
       </c>
       <c r="B10" s="6">
-        <v>0.727248278237558</v>
+        <v>0.605997583827389</v>
       </c>
       <c r="C10" s="6">
-        <v>0.77616436600000005</v>
+        <v>0.73835682844333095</v>
       </c>
       <c r="D10" s="1"/>
     </row>
-    <row r="11" spans="1:6" ht="20" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" ht="20">
       <c r="A11" s="5" t="s">
         <v>12</v>
       </c>
@@ -601,7 +606,7 @@
       </c>
       <c r="D11" s="1"/>
     </row>
-    <row r="12" spans="1:6" ht="20" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" ht="20">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>

</xml_diff>